<commit_message>
[Features] [2/12/2024] [Show latest income/outcome]
</commit_message>
<xml_diff>
--- a/bin/Debug/net8.0-windows10.0.19041.0/win10-x64/Data/Test.xlsx
+++ b/bin/Debug/net8.0-windows10.0.19041.0/win10-x64/Data/Test.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Date</t>
   </si>
@@ -31,6 +31,12 @@
     <t>Note</t>
   </si>
   <si>
+    <t>Timestamp</t>
+  </si>
+  <si>
+    <t>Summary</t>
+  </si>
+  <si>
     <t>Income</t>
   </si>
   <si>
@@ -44,6 +50,9 @@
   </si>
   <si>
     <t>Debt</t>
+  </si>
+  <si>
+    <t>Choose outcome category</t>
   </si>
 </sst>
 </file>
@@ -93,6 +102,204 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr codeName=""/>
+  <dimension ref="A1:G8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="11.115263938903809" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" customWidth="1"/>
+    <col min="3" max="3" width="23.621213912963867" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" customWidth="1"/>
+    <col min="6" max="6" width="11.115263938903809" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1">
+        <v>45628</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="0">
+        <v>1234</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="1">
+        <v>45628.824521030096</v>
+      </c>
+      <c r="G2" s="0">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1">
+        <v>45628</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="0">
+        <v>234</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="1">
+        <v>45628.82490107639</v>
+      </c>
+      <c r="G3" s="0">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1">
+        <v>45628</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="0">
+        <v>30000</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="1">
+        <v>45628.82509895833</v>
+      </c>
+      <c r="G4" s="0">
+        <v>31000</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1">
+        <v>45628</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="0">
+        <v>130000</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="1">
+        <v>45628.825217164354</v>
+      </c>
+      <c r="G5" s="0">
+        <v>-99000</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1">
+        <v>45628</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="0">
+        <v>12341</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="1">
+        <v>45628.88678170139</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1">
+        <v>45628</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="0">
+        <v>9000</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="1">
+        <v>45628.920668425926</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1">
+        <v>45628</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="0">
+        <v>1</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="1">
+        <v>45628.93586479167</v>
+      </c>
+    </row>
+  </sheetData>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr codeName=""/>
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -103,7 +310,7 @@
     <col min="2" max="2" width="9.140625" customWidth="1"/>
     <col min="3" max="3" width="9.140625" customWidth="1"/>
     <col min="4" max="4" width="9.140625" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" customWidth="1"/>
+    <col min="5" max="5" width="11.115263938903809" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -111,84 +318,84 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1">
-        <v>45624</v>
+        <v>45628</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="0">
+        <v>8</v>
+      </c>
+      <c r="C2" s="0">
         <v>1234</v>
       </c>
-      <c r="E2" s="0" t="s">
-        <v>7</v>
+      <c r="D2" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="1">
+        <v>45628.82452101852</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1">
-        <v>45625</v>
+        <v>45628</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="0">
-        <v>3456</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="C3" s="0">
+        <v>30000</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="1">
+        <v>45628.82509895833</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1">
-        <v>45624</v>
+        <v>45628</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="0">
-        <v>5678</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>7</v>
+      <c r="C4" s="0">
+        <v>12341</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="1">
+        <v>45628.88678170139</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1">
-        <v>45624</v>
+        <v>45628</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="0">
-        <v>1234</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="C5" s="0">
+        <v>9000</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="1">
+        <v>45628.920668425926</v>
       </c>
     </row>
   </sheetData>
@@ -196,19 +403,20 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr codeName=""/>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.115263938903809" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" customWidth="1"/>
+    <col min="2" max="2" width="23.621213912963867" customWidth="1"/>
     <col min="3" max="3" width="9.140625" customWidth="1"/>
     <col min="4" max="4" width="9.140625" customWidth="1"/>
+    <col min="5" max="5" width="11.115263938903809" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -224,89 +432,59 @@
       <c r="D1" s="0" t="s">
         <v>4</v>
       </c>
+      <c r="E1" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1">
-        <v>45624</v>
+        <v>45628</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C2" s="0">
-        <v>1234</v>
+        <v>234</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>7</v>
+        <v>9</v>
+      </c>
+      <c r="E2" s="1">
+        <v>45628.82490107639</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1">
-        <v>45625</v>
+        <v>45628</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C3" s="0">
-        <v>3456</v>
+        <v>130000</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>7</v>
+        <v>9</v>
+      </c>
+      <c r="E3" s="1">
+        <v>45628.825217164354</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1">
-        <v>45624</v>
+        <v>45628</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C4" s="0">
-        <v>1234</v>
+        <v>1</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>7</v>
-      </c>
-    </row>
-  </sheetData>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr codeName=""/>
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1">
-        <v>45624</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="0">
-        <v>5678</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>7</v>
+        <v>9</v>
+      </c>
+      <c r="E4" s="1">
+        <v>45628.93586479167</v>
       </c>
     </row>
   </sheetData>

</xml_diff>